<commit_message>
read force move effect config ok
</commit_message>
<xml_diff>
--- a/Data/Config/excel/effect/effects.xlsx
+++ b/Data/Config/excel/effect/effects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19455" windowHeight="8550" activeTab="1"/>
+    <workbookView windowWidth="26805" windowHeight="10950" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="effect_group" sheetId="5" r:id="rId1"/>
@@ -346,38 +346,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -390,9 +367,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -406,14 +390,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -423,46 +399,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -482,8 +418,72 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -498,7 +498,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -513,13 +513,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,31 +621,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,31 +645,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,97 +687,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,6 +704,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -717,30 +732,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -763,10 +754,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -782,16 +771,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -804,6 +793,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -812,10 +812,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -824,133 +824,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1309,7 +1309,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B$1:B$1048576"/>
+      <selection activeCell="D4" sqref="D$1:D$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1458,8 +1458,8 @@
   <sheetPr/>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1586,7 +1586,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C1" sqref="C$1:C$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1706,7 +1706,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B$1:B$1048576"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1999,7 +1999,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C$1:C$1048576"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -2124,8 +2124,8 @@
   <sheetPr/>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
try behaviac and try to use guided missile
</commit_message>
<xml_diff>
--- a/Data/Config/excel/effect/effects.xlsx
+++ b/Data/Config/excel/effect/effects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="13650" activeTab="6"/>
+    <workbookView windowWidth="27765" windowHeight="13650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="effect_group" sheetId="5" r:id="rId1"/>
@@ -353,9 +353,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -366,6 +366,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -373,30 +402,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -410,14 +425,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -433,72 +487,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -509,6 +502,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -519,187 +519,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,24 +710,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -757,15 +739,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -802,6 +775,33 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -818,145 +818,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1466,8 +1466,8 @@
   <sheetPr/>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1578,8 +1578,8 @@
       <c r="B17">
         <v>1000004</v>
       </c>
-      <c r="C17" t="s">
-        <v>24</v>
+      <c r="C17">
+        <v>1000001</v>
       </c>
     </row>
   </sheetData>
@@ -1594,7 +1594,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -2278,7 +2278,7 @@
   <sheetPr/>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change filter anchor enum and force move anchor enum
</commit_message>
<xml_diff>
--- a/Data/Config/excel/effect/effects.xlsx
+++ b/Data/Config/excel/effect/effects.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="13650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13650" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="effect_group" sheetId="5" r:id="rId1"/>
@@ -34,18 +34,15 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t>Administrator:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-pos 坐标
-owner effect释放者
-target：Effect目标</t>
+          <t>target_pos 技能目标位置
+target_unit 技能目标
+caster 技能释放者
+cast_pos 技能施放时位置
+effect_target_unit 效果目标
+effect_target_pos效果目标位置
+effect_dir 效果方向
+skill_dir 技能方向
+cast_face_dir 技能施放时su朝向</t>
         </r>
       </text>
     </comment>
@@ -54,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="97">
   <si>
     <t>效果id</t>
   </si>
@@ -332,32 +329,29 @@
     <t>ts;3000;3</t>
   </si>
   <si>
-    <t>owner</t>
-  </si>
-  <si>
     <t>td;3000;6</t>
   </si>
   <si>
-    <t>target</t>
-  </si>
-  <si>
     <t>sd;3;9</t>
   </si>
   <si>
-    <t>pos</t>
+    <t>caster</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>target_unit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>effect_target_unit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,345 +360,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -712,251 +388,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -965,57 +399,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1306,19 +693,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -1330,12 +717,12 @@
     <col min="10" max="10" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="1" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" customFormat="1" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1375,7 +762,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="1" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1395,7 +782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="1" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>4000001</v>
       </c>
@@ -1415,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>4000002</v>
       </c>
@@ -1435,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="1" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>4000003</v>
       </c>
@@ -1456,21 +843,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="26.625" customWidth="1"/>
@@ -1481,20 +867,12 @@
     <col min="7" max="7" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="1"/>
-    <row r="3" customFormat="1"/>
-    <row r="4" customFormat="1"/>
-    <row r="5" customFormat="1"/>
-    <row r="6" customFormat="1"/>
-    <row r="7" customFormat="1"/>
-    <row r="8" customFormat="1"/>
-    <row r="9" customFormat="1"/>
-    <row r="10" customFormat="1" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +883,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" customFormat="1" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1516,7 +894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" customFormat="1" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1527,7 +905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" customFormat="1" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>7000001</v>
       </c>
@@ -1538,7 +916,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>7000002</v>
       </c>
@@ -1549,7 +927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" customFormat="1" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>7000003</v>
       </c>
@@ -1560,7 +938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" customFormat="1" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>7000004</v>
       </c>
@@ -1571,7 +949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" customFormat="1" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>7000005</v>
       </c>
@@ -1583,21 +961,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -1608,12 +985,12 @@
     <col min="7" max="7" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1624,7 +1001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1635,7 +1012,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1646,7 +1023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1000001</v>
       </c>
@@ -1657,7 +1034,7 @@
         <v>1000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1000002</v>
       </c>
@@ -1668,7 +1045,7 @@
         <v>1000002</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1000003</v>
       </c>
@@ -1679,7 +1056,7 @@
         <v>1000003</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1000004</v>
       </c>
@@ -1690,7 +1067,7 @@
         <v>1000004</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>1000005</v>
       </c>
@@ -1702,22 +1079,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="5" width="36" customWidth="1"/>
@@ -1727,12 +1103,12 @@
     <col min="10" max="10" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="1" spans="1:6">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1752,7 +1128,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" customFormat="1" spans="1:6">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1772,7 +1148,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" customFormat="1" spans="1:6">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1792,7 +1168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="1" spans="1:6">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>3000001</v>
       </c>
@@ -1812,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="1:8">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>3000002</v>
       </c>
@@ -1835,7 +1211,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" customFormat="1" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>3000003</v>
       </c>
@@ -1861,7 +1237,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="8:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="H16" t="s">
         <v>41</v>
       </c>
@@ -1869,7 +1245,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="8:12">
+    <row r="17" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H17" t="s">
         <v>43</v>
       </c>
@@ -1877,7 +1253,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="8:12">
+    <row r="18" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H18" t="s">
         <v>45</v>
       </c>
@@ -1885,7 +1261,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="8:11">
+    <row r="19" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H19" t="s">
         <v>47</v>
       </c>
@@ -1893,7 +1269,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="8:10">
+    <row r="20" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H20" t="s">
         <v>49</v>
       </c>
@@ -1901,7 +1277,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="8:10">
+    <row r="21" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H21" t="s">
         <v>51</v>
       </c>
@@ -1909,7 +1285,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="8:10">
+    <row r="22" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H22" t="s">
         <v>53</v>
       </c>
@@ -1917,7 +1293,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="8:10">
+    <row r="23" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H23" t="s">
         <v>55</v>
       </c>
@@ -1925,7 +1301,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="8:11">
+    <row r="24" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H24" t="s">
         <v>57</v>
       </c>
@@ -1933,7 +1309,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="8:10">
+    <row r="25" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H25" t="s">
         <v>59</v>
       </c>
@@ -1941,7 +1317,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="8:10">
+    <row r="26" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H26" t="s">
         <v>61</v>
       </c>
@@ -1949,7 +1325,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="8:10">
+    <row r="27" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H27" t="s">
         <v>63</v>
       </c>
@@ -1957,7 +1333,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="8:11">
+    <row r="29" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H29" t="s">
         <v>65</v>
       </c>
@@ -1965,7 +1341,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="8:11">
+    <row r="30" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H30" t="s">
         <v>67</v>
       </c>
@@ -1973,7 +1349,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="8:12">
+    <row r="31" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H31" t="s">
         <v>69</v>
       </c>
@@ -1981,7 +1357,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="8:10">
+    <row r="32" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H32" t="s">
         <v>71</v>
       </c>
@@ -1989,28 +1365,27 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="8:8">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.15">
       <c r="H34" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -2020,20 +1395,12 @@
     <col min="6" max="6" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="1"/>
-    <row r="3" customFormat="1"/>
-    <row r="4" customFormat="1"/>
-    <row r="5" customFormat="1"/>
-    <row r="6" customFormat="1"/>
-    <row r="7" customFormat="1"/>
-    <row r="8" customFormat="1"/>
-    <row r="9" customFormat="1"/>
-    <row r="10" customFormat="1" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2044,7 +1411,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" customFormat="1" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2055,7 +1422,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" customFormat="1" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2066,7 +1433,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" customFormat="1" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>5000001</v>
       </c>
@@ -2077,7 +1444,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>5000002</v>
       </c>
@@ -2088,7 +1455,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" customFormat="1" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>5000003</v>
       </c>
@@ -2099,7 +1466,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" customFormat="1" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>5000004</v>
       </c>
@@ -2110,7 +1477,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" customFormat="1" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>5000005</v>
       </c>
@@ -2122,21 +1489,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="4" width="36" customWidth="1"/>
@@ -2147,24 +1513,17 @@
     <col min="9" max="9" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="1"/>
-    <row r="3" customFormat="1"/>
-    <row r="4" customFormat="1"/>
-    <row r="5" customFormat="1"/>
-    <row r="6" customFormat="1"/>
-    <row r="7" customFormat="1"/>
-    <row r="8" customFormat="1"/>
-    <row r="9" customFormat="1" spans="3:3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" customFormat="1" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2181,7 +1540,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" customFormat="1" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2198,7 +1557,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" customFormat="1" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2215,7 +1574,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" customFormat="1" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>6000001</v>
       </c>
@@ -2226,13 +1585,13 @@
         <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>6000002</v>
       </c>
@@ -2240,16 +1599,16 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E14">
         <v>180</v>
       </c>
     </row>
-    <row r="15" customFormat="1" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>6000003</v>
       </c>
@@ -2257,7 +1616,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
@@ -2267,22 +1626,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -2293,12 +1651,12 @@
     <col min="7" max="7" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="1" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2306,7 +1664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" customFormat="1" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2314,7 +1672,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" customFormat="1" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2322,7 +1680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="1" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2000001</v>
       </c>
@@ -2330,7 +1688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2000002</v>
       </c>
@@ -2338,7 +1696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="1" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2000003</v>
       </c>
@@ -2347,8 +1705,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improve scene script subscribe scene events
</commit_message>
<xml_diff>
--- a/Data/Config/excel/effect/effects.xlsx
+++ b/Data/Config/excel/effect/effects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="13650" activeTab="1"/>
+    <workbookView windowWidth="27765" windowHeight="13230" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="effect_group" sheetId="5" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103">
   <si>
     <t>效果id</t>
   </si>
@@ -278,13 +278,37 @@
     <t>class_name</t>
   </si>
   <si>
-    <t>script_param</t>
+    <t>str_param</t>
+  </si>
+  <si>
+    <t>json_param</t>
+  </si>
+  <si>
+    <t>int_param</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
     <t>effect_script.effect_script_demo</t>
+  </si>
+  <si>
+    <t>str_1</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>str_2</t>
+  </si>
+  <si>
+    <t>str_3</t>
+  </si>
+  <si>
+    <t>str_4</t>
+  </si>
+  <si>
+    <t>str_5</t>
   </si>
   <si>
     <t>备注：t时间毫秒 d距离 s速度。知道任意2个可以推导出第三个。</t>
@@ -343,10 +367,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -357,29 +381,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
@@ -387,16 +388,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -410,16 +411,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -439,9 +432,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -457,49 +503,27 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -510,187 +534,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -701,41 +725,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -769,6 +758,44 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -784,20 +811,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -809,10 +833,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -821,133 +845,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1457,7 +1481,7 @@
   <sheetPr/>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1987,13 +2011,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -2008,7 +2032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2018,8 +2042,14 @@
       <c r="C10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2029,71 +2059,113 @@
       <c r="C11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>5000001</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>5000002</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>82</v>
+      </c>
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>5000003</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>5000004</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>84</v>
+      </c>
+      <c r="D16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>5000005</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2129,7 +2201,7 @@
     </row>
     <row r="9" spans="3:3">
       <c r="C9" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2137,16 +2209,16 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2154,16 +2226,16 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2171,16 +2243,16 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2191,10 +2263,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2208,10 +2280,10 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E14">
         <v>180</v>
@@ -2225,10 +2297,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E15">
         <v>90</v>

</xml_diff>

<commit_message>
modify lua to make it more clear
</commit_message>
<xml_diff>
--- a/Data/Config/excel/effect/effects.xlsx
+++ b/Data/Config/excel/effect/effects.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="13230" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13230" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="effect_group" sheetId="5" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
   <si>
     <t>效果id</t>
   </si>
@@ -290,9 +290,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>effect_script.effect_script_demo</t>
-  </si>
-  <si>
     <t>str_1</t>
   </si>
   <si>
@@ -360,19 +357,17 @@
   </si>
   <si>
     <t>effect_target_unit</t>
+  </si>
+  <si>
+    <t>effect_script.effect_demo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,345 +376,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -727,251 +404,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -980,57 +415,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1321,19 +709,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -1345,12 +733,12 @@
     <col min="10" max="10" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1370,7 +758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1390,7 +778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1410,7 +798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>4000001</v>
       </c>
@@ -1430,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>4000002</v>
       </c>
@@ -1450,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>4000003</v>
       </c>
@@ -1471,21 +859,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="26.625" customWidth="1"/>
@@ -1496,12 +883,12 @@
     <col min="7" max="7" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1512,7 +899,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1523,7 +910,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1534,7 +921,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>7000001</v>
       </c>
@@ -1545,7 +932,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>7000002</v>
       </c>
@@ -1556,7 +943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>7000003</v>
       </c>
@@ -1567,7 +954,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>7000004</v>
       </c>
@@ -1578,7 +965,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>7000005</v>
       </c>
@@ -1590,21 +977,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -1615,12 +1001,12 @@
     <col min="7" max="7" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1631,7 +1017,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1642,7 +1028,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1653,7 +1039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1000001</v>
       </c>
@@ -1664,7 +1050,7 @@
         <v>1000001</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1000002</v>
       </c>
@@ -1675,7 +1061,7 @@
         <v>1000002</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1000003</v>
       </c>
@@ -1686,7 +1072,7 @@
         <v>1000003</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1000004</v>
       </c>
@@ -1697,7 +1083,7 @@
         <v>1000004</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>1000005</v>
       </c>
@@ -1709,22 +1095,21 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="5" width="36" customWidth="1"/>
@@ -1734,12 +1119,12 @@
     <col min="10" max="10" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1759,7 +1144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1779,7 +1164,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1799,7 +1184,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>3000001</v>
       </c>
@@ -1819,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>3000002</v>
       </c>
@@ -1842,7 +1227,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>3000003</v>
       </c>
@@ -1868,7 +1253,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="8:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="H16" t="s">
         <v>39</v>
       </c>
@@ -1876,7 +1261,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="8:12">
+    <row r="17" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H17" t="s">
         <v>41</v>
       </c>
@@ -1884,7 +1269,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="8:12">
+    <row r="18" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H18" t="s">
         <v>43</v>
       </c>
@@ -1892,7 +1277,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="8:11">
+    <row r="19" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H19" t="s">
         <v>45</v>
       </c>
@@ -1900,7 +1285,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="8:10">
+    <row r="20" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H20" t="s">
         <v>47</v>
       </c>
@@ -1908,7 +1293,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="8:10">
+    <row r="21" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H21" t="s">
         <v>49</v>
       </c>
@@ -1916,7 +1301,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="8:10">
+    <row r="22" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H22" t="s">
         <v>51</v>
       </c>
@@ -1924,7 +1309,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="8:10">
+    <row r="23" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H23" t="s">
         <v>53</v>
       </c>
@@ -1932,7 +1317,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="8:11">
+    <row r="24" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H24" t="s">
         <v>55</v>
       </c>
@@ -1940,7 +1325,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="8:10">
+    <row r="25" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H25" t="s">
         <v>57</v>
       </c>
@@ -1948,7 +1333,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="8:10">
+    <row r="26" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H26" t="s">
         <v>59</v>
       </c>
@@ -1956,7 +1341,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="8:10">
+    <row r="27" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H27" t="s">
         <v>61</v>
       </c>
@@ -1964,7 +1349,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="8:11">
+    <row r="29" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H29" t="s">
         <v>63</v>
       </c>
@@ -1972,7 +1357,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="8:11">
+    <row r="30" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H30" t="s">
         <v>65</v>
       </c>
@@ -1980,7 +1365,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="8:12">
+    <row r="31" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H31" t="s">
         <v>67</v>
       </c>
@@ -1988,7 +1373,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="8:10">
+    <row r="32" spans="8:12" x14ac:dyDescent="0.15">
       <c r="H32" t="s">
         <v>69</v>
       </c>
@@ -1996,28 +1381,27 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="8:8">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.15">
       <c r="H34" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -2027,12 +1411,12 @@
     <col min="6" max="6" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2049,7 +1433,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2066,7 +1450,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2083,107 +1467,106 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>5000001</v>
       </c>
       <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
         <v>79</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>80</v>
-      </c>
-      <c r="D13" t="s">
-        <v>81</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>5000002</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>5000003</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>5000004</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>5000005</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="4" width="36" customWidth="1"/>
@@ -2194,56 +1577,56 @@
     <col min="9" max="9" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="3:3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
         <v>87</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>88</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>89</v>
       </c>
-      <c r="E10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" t="s">
         <v>91</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>92</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>93</v>
       </c>
-      <c r="E11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
         <v>78</v>
@@ -2252,10 +1635,10 @@
         <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>6000001</v>
       </c>
@@ -2263,16 +1646,16 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
         <v>97</v>
-      </c>
-      <c r="D13" t="s">
-        <v>98</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>6000002</v>
       </c>
@@ -2280,16 +1663,16 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" t="s">
         <v>99</v>
-      </c>
-      <c r="D14" t="s">
-        <v>100</v>
       </c>
       <c r="E14">
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>6000003</v>
       </c>
@@ -2297,32 +1680,31 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
         <v>101</v>
-      </c>
-      <c r="D15" t="s">
-        <v>102</v>
       </c>
       <c r="E15">
         <v>90</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.625" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -2333,12 +1715,12 @@
     <col min="7" max="7" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2346,7 +1728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2354,7 +1736,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2362,7 +1744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2000001</v>
       </c>
@@ -2370,7 +1752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2000002</v>
       </c>
@@ -2378,7 +1760,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2000003</v>
       </c>
@@ -2387,8 +1769,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>